<commit_message>
Modified the Build sequences script for GraphAligner
</commit_message>
<xml_diff>
--- a/Results and findings/Sequence Edit Distance/FinalResults/MatchRate.xlsx
+++ b/Results and findings/Sequence Edit Distance/FinalResults/MatchRate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusreen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusreen/Documents/GitHub/Thesis/Results and findings/Sequence Edit Distance/FinalResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11E28A3-6CD8-2949-A861-20CEE2F496B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68835DAA-773F-8644-B145-D09E1C9447F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" activeTab="3" xr2:uid="{7934335E-4B17-0B47-8C68-450A467D6623}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" activeTab="1" xr2:uid="{7934335E-4B17-0B47-8C68-450A467D6623}"/>
   </bookViews>
   <sheets>
     <sheet name="111" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,7 @@
     <sheet name="CAMIH1" sheetId="3" r:id="rId3"/>
     <sheet name="Real" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.10" hidden="1">Real!$F$57</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Real!$F$58:$F$68</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Real!$G$57</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Real!$G$58:$G$68</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Real!$H$57</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Real!$H$58:$H$68</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Real!$E$57</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Real!$E$58:$E$68</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Real!$E$57</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Real!$E$58:$E$68</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Real!$F$57</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Real!$F$58:$F$68</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Real!$G$57</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Real!$G$58:$G$68</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">Real!$H$57</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">Real!$H$58:$H$68</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="20">
   <si>
     <t>EditDistance_GraphAligner_Query</t>
   </si>
@@ -150,6 +132,12 @@
   </si>
   <si>
     <t>Frequency GraphALIGNER</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Frequency</t>
   </si>
 </sst>
 </file>
@@ -249,17 +237,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,7 +1158,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3.7037037037037033</c:v>
+                  <c:v>3.6363636363636362</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1175,16 +1167,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7037037037037033</c:v>
+                  <c:v>3.6363636363636362</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.814814814814813</c:v>
+                  <c:v>16.363636363636363</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.962962962962962</c:v>
+                  <c:v>61.818181818181813</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.2592592592592595</c:v>
+                  <c:v>9.0909090909090917</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1196,7 +1188,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5555555555555554</c:v>
+                  <c:v>5.4545454545454541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6083,10 +6075,10 @@
       <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K15" t="s">
@@ -6103,10 +6095,10 @@
       <c r="C16" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="I16" s="3">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
@@ -6123,10 +6115,10 @@
       <c r="C17" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17">
         <v>0.1</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17">
         <v>7</v>
       </c>
       <c r="K17">
@@ -6144,10 +6136,10 @@
       <c r="C18" s="2">
         <v>0.99303135888501703</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18">
         <v>0.2</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
@@ -6165,10 +6157,10 @@
       <c r="C19" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19">
         <v>0.3</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
@@ -6186,10 +6178,10 @@
       <c r="C20" s="2">
         <v>0.99102564102564095</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20">
         <v>0.4</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
@@ -6207,10 +6199,10 @@
       <c r="C21" s="2">
         <v>0.992307692307692</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21">
         <v>0.5</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21">
         <v>2</v>
       </c>
       <c r="K21">
@@ -6228,10 +6220,10 @@
       <c r="C22" s="2">
         <v>0.99102564102564095</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22">
         <v>0.6</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22">
         <v>3</v>
       </c>
       <c r="K22">
@@ -6249,10 +6241,10 @@
       <c r="C23" s="2">
         <v>0.99358974358974395</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23">
         <v>0.7</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
@@ -6270,10 +6262,10 @@
       <c r="C24" s="2">
         <v>0.992307692307692</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24">
         <v>0.8</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
@@ -6291,10 +6283,10 @@
       <c r="C25" s="2">
         <v>0.989547038327526</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25">
         <v>0.9</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
@@ -6312,10 +6304,10 @@
       <c r="C26" s="2">
         <v>0.99070847851335697</v>
       </c>
-      <c r="I26" s="3">
-        <v>1</v>
-      </c>
-      <c r="J26" s="4">
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
         <v>366</v>
       </c>
       <c r="K26">
@@ -6333,10 +6325,10 @@
       <c r="C27" s="2">
         <v>0.99419279907084801</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J27" s="3">
         <f>SUM(J16:J26)</f>
         <v>378</v>
       </c>
@@ -6373,10 +6365,10 @@
       <c r="C30" s="2">
         <v>0.99535423925667799</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="J30" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K30" t="s">
@@ -6393,10 +6385,10 @@
       <c r="C31" s="2">
         <v>0.99767711962833905</v>
       </c>
-      <c r="I31" s="3">
-        <v>0</v>
-      </c>
-      <c r="J31" s="4">
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
         <v>147</v>
       </c>
       <c r="K31">
@@ -6414,10 +6406,10 @@
       <c r="C32" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32">
         <v>0.1</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32">
         <v>0</v>
       </c>
       <c r="K32">
@@ -6435,10 +6427,10 @@
       <c r="C33" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33">
         <v>0.2</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33">
         <v>0</v>
       </c>
       <c r="K33">
@@ -6456,10 +6448,10 @@
       <c r="C34" s="2">
         <v>0.99767711962833905</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34">
         <v>0.3</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34">
         <v>0</v>
       </c>
       <c r="K34">
@@ -6477,10 +6469,10 @@
       <c r="C35" s="2">
         <v>0.99303135888501703</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35">
         <v>0.4</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35">
         <v>0</v>
       </c>
       <c r="K35">
@@ -6498,10 +6490,10 @@
       <c r="C36" s="2">
         <v>0.99303135888501703</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36">
         <v>0.5</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36">
         <v>0</v>
       </c>
       <c r="K36">
@@ -6519,10 +6511,10 @@
       <c r="C37" s="2">
         <v>0.99070847851335697</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37">
         <v>0.6</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37">
         <v>1</v>
       </c>
       <c r="K37">
@@ -6540,10 +6532,10 @@
       <c r="C38" s="2">
         <v>0.99303135888501703</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38">
         <v>0.7</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38">
         <v>0</v>
       </c>
       <c r="K38">
@@ -6561,10 +6553,10 @@
       <c r="C39" s="2">
         <v>0.989547038327526</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39">
         <v>0.8</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39">
         <v>0</v>
       </c>
       <c r="K39">
@@ -6582,10 +6574,10 @@
       <c r="C40" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40">
         <v>0.9</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40">
         <v>0</v>
       </c>
       <c r="K40">
@@ -6603,10 +6595,10 @@
       <c r="C41" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="I41" s="3">
-        <v>1</v>
-      </c>
-      <c r="J41" s="4">
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
         <v>230</v>
       </c>
       <c r="K41">
@@ -6624,10 +6616,10 @@
       <c r="C42" s="2">
         <v>0.989547038327526</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J42" s="5">
+      <c r="J42" s="3">
         <v>378</v>
       </c>
     </row>
@@ -6663,10 +6655,10 @@
       <c r="C45" s="2">
         <v>0.99419279907084801</v>
       </c>
-      <c r="I45" s="6" t="s">
+      <c r="I45" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J45" s="6" t="s">
+      <c r="J45" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K45" t="s">
@@ -6683,10 +6675,10 @@
       <c r="C46" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="I46" s="3">
-        <v>0</v>
-      </c>
-      <c r="J46" s="4">
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
         <v>0</v>
       </c>
       <c r="K46">
@@ -6704,10 +6696,10 @@
       <c r="C47" s="2">
         <v>0.99535423925667799</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47">
         <v>0.1</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J47">
         <v>0</v>
       </c>
       <c r="K47">
@@ -6725,10 +6717,10 @@
       <c r="C48" s="2">
         <v>0.99535423925667799</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48">
         <v>0.2</v>
       </c>
-      <c r="J48" s="4">
+      <c r="J48">
         <v>0</v>
       </c>
       <c r="K48">
@@ -6746,10 +6738,10 @@
       <c r="C49" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49">
         <v>0.3</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J49">
         <v>0</v>
       </c>
       <c r="K49">
@@ -6767,10 +6759,10 @@
       <c r="C50" s="2">
         <v>0.99419279907084801</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50">
         <v>0.4</v>
       </c>
-      <c r="J50" s="4">
+      <c r="J50">
         <v>0</v>
       </c>
       <c r="K50">
@@ -6788,10 +6780,10 @@
       <c r="C51" s="2">
         <v>0.99639639639639599</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51">
         <v>0.5</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51">
         <v>3</v>
       </c>
       <c r="K51">
@@ -6809,10 +6801,10 @@
       <c r="C52" s="2">
         <v>0.99303135888501703</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52">
         <v>0.6</v>
       </c>
-      <c r="J52" s="4">
+      <c r="J52">
         <v>3</v>
       </c>
       <c r="K52">
@@ -6830,10 +6822,10 @@
       <c r="C53" s="2">
         <v>0.989547038327526</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53">
         <v>0.7</v>
       </c>
-      <c r="J53" s="4">
+      <c r="J53">
         <v>0</v>
       </c>
       <c r="K53">
@@ -6851,10 +6843,10 @@
       <c r="C54" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54">
         <v>0.8</v>
       </c>
-      <c r="J54" s="4">
+      <c r="J54">
         <v>0</v>
       </c>
       <c r="K54">
@@ -6872,10 +6864,10 @@
       <c r="C55" s="2">
         <v>0.989547038327526</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55">
         <v>0.9</v>
       </c>
-      <c r="J55" s="4">
+      <c r="J55">
         <v>0</v>
       </c>
       <c r="K55">
@@ -6893,10 +6885,10 @@
       <c r="C56" s="2">
         <v>0.98606271777003496</v>
       </c>
-      <c r="I56" s="3">
-        <v>1</v>
-      </c>
-      <c r="J56" s="4">
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
         <v>372</v>
       </c>
       <c r="K56">
@@ -6914,10 +6906,10 @@
       <c r="C57" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="I57" s="5" t="s">
+      <c r="I57" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J57" s="5">
+      <c r="J57" s="3">
         <v>378</v>
       </c>
     </row>
@@ -6965,7 +6957,7 @@
       <c r="C60" s="2">
         <v>0.99419279907084801</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60">
         <v>0</v>
       </c>
       <c r="J60">
@@ -6976,7 +6968,7 @@
         <v>0</v>
       </c>
       <c r="L60">
-        <f>SUM($J60/$J$57)*100</f>
+        <f t="shared" ref="L60:L70" si="3">SUM($J60/$J$57)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -6990,7 +6982,7 @@
       <c r="C61" s="2">
         <v>0.99419279907084801</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61">
         <v>0.1</v>
       </c>
       <c r="J61">
@@ -6998,11 +6990,11 @@
         <v>1.8518518518518516</v>
       </c>
       <c r="K61">
-        <f t="shared" ref="K61:K70" ca="1" si="3">($J61/$J$42)*100</f>
+        <f t="shared" ref="K61:K70" ca="1" si="4">($J61/$J$42)*100</f>
         <v>0</v>
       </c>
       <c r="L61">
-        <f ca="1">SUM($J61/$J$57)*100</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7016,19 +7008,19 @@
       <c r="C62" s="2">
         <v>0.99070847851335697</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62">
         <v>0.2</v>
       </c>
       <c r="J62">
-        <f t="shared" ref="J62:J70" ca="1" si="4">($J62/$J$27)*100</f>
+        <f t="shared" ref="J62:J70" ca="1" si="5">($J62/$J$27)*100</f>
         <v>0</v>
       </c>
       <c r="K62">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L62">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L62">
-        <f ca="1">SUM($J62/$J$57)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -7042,19 +7034,19 @@
       <c r="C63" s="2">
         <v>0.99070847851335697</v>
       </c>
-      <c r="I63" s="3">
+      <c r="I63">
         <v>0.3</v>
       </c>
       <c r="J63">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K63">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="K63">
+      <c r="L63">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L63">
-        <f ca="1">SUM($J63/$J$57)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -7068,19 +7060,19 @@
       <c r="C64" s="2">
         <v>0.99303135888501703</v>
       </c>
-      <c r="I64" s="3">
+      <c r="I64">
         <v>0.4</v>
       </c>
       <c r="J64">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K64">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="K64">
+      <c r="L64">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L64">
-        <f ca="1">SUM($J64/$J$57)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -7094,19 +7086,19 @@
       <c r="C65" s="2">
         <v>0.99368686868686895</v>
       </c>
-      <c r="I65" s="3">
+      <c r="I65">
         <v>0.5</v>
       </c>
       <c r="J65">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.52910052910052907</v>
+      </c>
+      <c r="K65">
         <f t="shared" ca="1" si="4"/>
-        <v>0.52910052910052907</v>
-      </c>
-      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L65">
-        <f ca="1">SUM($J65/$J$57)*100</f>
         <v>0.79365079365079361</v>
       </c>
     </row>
@@ -7120,19 +7112,19 @@
       <c r="C66" s="2">
         <v>0.99761904761904796</v>
       </c>
-      <c r="I66" s="3">
+      <c r="I66">
         <v>0.6</v>
       </c>
       <c r="J66">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.79365079365079361</v>
+      </c>
+      <c r="K66">
         <f t="shared" ca="1" si="4"/>
-        <v>0.79365079365079361</v>
-      </c>
-      <c r="K66">
+        <v>0.26455026455026454</v>
+      </c>
+      <c r="L66">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26455026455026454</v>
-      </c>
-      <c r="L66">
-        <f ca="1">SUM($J66/$J$57)*100</f>
         <v>0.79365079365079361</v>
       </c>
     </row>
@@ -7146,19 +7138,19 @@
       <c r="C67" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I67">
         <v>0.7</v>
       </c>
       <c r="J67">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K67">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="K67">
+      <c r="L67">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L67">
-        <f ca="1">SUM($J67/$J$57)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -7172,19 +7164,19 @@
       <c r="C68" s="2">
         <v>0.95151515151515198</v>
       </c>
-      <c r="I68" s="3">
+      <c r="I68">
         <v>0.8</v>
       </c>
       <c r="J68">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K68">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="K68">
+      <c r="L68">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L68">
-        <f ca="1">SUM($J68/$J$57)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -7198,19 +7190,19 @@
       <c r="C69" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="I69" s="3">
+      <c r="I69">
         <v>0.9</v>
       </c>
       <c r="J69">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K69">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L69">
-        <f ca="1">SUM($J69/$J$57)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -7224,19 +7216,19 @@
       <c r="C70" s="2">
         <v>0.99070847851335697</v>
       </c>
-      <c r="I70" s="3">
+      <c r="I70">
         <v>1</v>
       </c>
       <c r="J70">
+        <f t="shared" ca="1" si="5"/>
+        <v>96.825396825396822</v>
+      </c>
+      <c r="K70">
         <f t="shared" ca="1" si="4"/>
-        <v>96.825396825396822</v>
-      </c>
-      <c r="K70">
+        <v>60.846560846560848</v>
+      </c>
+      <c r="L70">
         <f t="shared" ca="1" si="3"/>
-        <v>60.846560846560848</v>
-      </c>
-      <c r="L70">
-        <f ca="1">SUM($J70/$J$57)*100</f>
         <v>98.412698412698404</v>
       </c>
     </row>
@@ -10650,10 +10642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD53D70E-726F-7545-8E44-B7765AB9F7C2}">
-  <dimension ref="A1:J379"/>
+  <dimension ref="A1:M379"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G12"/>
+    <sheetView tabSelected="1" topLeftCell="B75" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10666,7 +10658,7 @@
     <col min="9" max="9" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10680,7 +10672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0.49081364829396301</v>
       </c>
@@ -10694,7 +10686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0.34851138353765299</v>
       </c>
@@ -10708,7 +10700,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0.32049036777583201</v>
       </c>
@@ -10722,7 +10714,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0.44563918757467103</v>
       </c>
@@ -10736,7 +10728,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0.38302277432712201</v>
       </c>
@@ -10750,7 +10742,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0.47260273972602701</v>
       </c>
@@ -10764,7 +10756,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0.50119617224880397</v>
       </c>
@@ -10778,7 +10770,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0.49068322981366502</v>
       </c>
@@ -10792,7 +10784,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>0.48497409326424901</v>
       </c>
@@ -10806,7 +10798,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>0.413020833333333</v>
       </c>
@@ -10820,7 +10812,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>0.45595854922279799</v>
       </c>
@@ -10834,7 +10826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>0.460103626943005</v>
       </c>
@@ -10848,7 +10840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>0.488843813387424</v>
       </c>
@@ -10859,7 +10851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>0.91923076923076896</v>
       </c>
@@ -10869,17 +10861,23 @@
       <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>0.50135501355013601</v>
       </c>
@@ -10889,18 +10887,24 @@
       <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>2</v>
       </c>
       <c r="I16">
         <f>($H16/$H$27)*100</f>
-        <v>3.7037037037037033</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6363636363636362</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>0.48888888888888898</v>
       </c>
@@ -10910,18 +10914,24 @@
       <c r="C17" s="2">
         <v>1</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17">
         <v>0.1</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
         <f t="shared" ref="I17:I26" si="0">($H17/$H$27)*100</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L17" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="M17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>0.2878257487359</v>
       </c>
@@ -10931,18 +10941,24 @@
       <c r="C18" s="2">
         <v>1</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18">
         <v>0.2</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L18" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M18" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>0.91792929292929304</v>
       </c>
@@ -10952,18 +10968,24 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <v>0.3</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19">
         <v>2</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>3.7037037037037033</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.6363636363636362</v>
+      </c>
+      <c r="L19" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="M19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>0.58501314636283996</v>
       </c>
@@ -10973,18 +10995,24 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20">
         <v>0.4</v>
       </c>
-      <c r="H20" s="4">
-        <v>8</v>
+      <c r="H20">
+        <v>9</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>14.814814814814813</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>16.363636363636363</v>
+      </c>
+      <c r="L20" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="M20" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>0.48100172711571698</v>
       </c>
@@ -10994,18 +11022,24 @@
       <c r="C21" s="2">
         <v>1</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21">
         <v>0.5</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21">
         <v>34</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>62.962962962962962</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>61.818181818181813</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="M21" s="7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>0.49678800856531002</v>
       </c>
@@ -11015,18 +11049,24 @@
       <c r="C22" s="2">
         <v>1</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22">
         <v>0.6</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22">
         <v>5</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>9.2592592592592595</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="L22" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="M22" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>0.37884314747264197</v>
       </c>
@@ -11036,18 +11076,24 @@
       <c r="C23" s="2">
         <v>1</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23">
         <v>0.7</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L23" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="M23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>0.37532671197072698</v>
       </c>
@@ -11057,18 +11103,24 @@
       <c r="C24" s="2">
         <v>1</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24">
         <v>0.8</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L24" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="M24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>0.458592132505176</v>
       </c>
@@ -11078,18 +11130,24 @@
       <c r="C25" s="2">
         <v>1</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25">
         <v>0.9</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L25" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="M25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>0.44927536231884102</v>
       </c>
@@ -11099,18 +11157,24 @@
       <c r="C26" s="2">
         <v>1</v>
       </c>
-      <c r="G26" s="3">
-        <v>1</v>
-      </c>
-      <c r="H26" s="4">
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
         <v>3</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>5.5555555555555554</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.4545454545454541</v>
+      </c>
+      <c r="L26" s="6">
+        <v>1</v>
+      </c>
+      <c r="M26" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>0.48208469055374598</v>
       </c>
@@ -11120,15 +11184,21 @@
       <c r="C27" s="2">
         <v>1</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="3">
         <f>SUM(H16:H26)</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>0.41610284167794298</v>
       </c>
@@ -11139,7 +11209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>0.494871794871795</v>
       </c>
@@ -11150,7 +11220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>0</v>
       </c>
@@ -11160,17 +11230,17 @@
       <c r="C30" s="2">
         <v>1</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>0.49679258731290099</v>
       </c>
@@ -11180,10 +11250,10 @@
       <c r="C31" s="2">
         <v>1</v>
       </c>
-      <c r="G31" s="3">
-        <v>0</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
         <v>0</v>
       </c>
       <c r="I31">
@@ -11191,7 +11261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>0.49347826086956498</v>
       </c>
@@ -11201,10 +11271,10 @@
       <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32">
         <v>0.1</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32">
         <v>0</v>
       </c>
       <c r="I32">
@@ -11222,10 +11292,10 @@
       <c r="C33" s="2">
         <v>1</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33">
         <v>0.2</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
@@ -11243,10 +11313,10 @@
       <c r="C34" s="2">
         <v>1</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34">
         <v>0.3</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
@@ -11264,10 +11334,10 @@
       <c r="C35" s="2">
         <v>1</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35">
         <v>0.4</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
@@ -11285,10 +11355,10 @@
       <c r="C36" s="2">
         <v>1</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36">
         <v>0.5</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36">
         <v>1</v>
       </c>
       <c r="I36">
@@ -11306,10 +11376,10 @@
       <c r="C37" s="2">
         <v>1</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37">
         <v>0.6</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37">
         <v>0</v>
       </c>
       <c r="I37">
@@ -11327,10 +11397,10 @@
       <c r="C38" s="2">
         <v>1</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38">
         <v>0.7</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38">
         <v>2</v>
       </c>
       <c r="I38">
@@ -11348,10 +11418,10 @@
       <c r="C39" s="2">
         <v>1</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39">
         <v>0.8</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39">
         <v>1</v>
       </c>
       <c r="I39">
@@ -11369,10 +11439,10 @@
       <c r="C40" s="2">
         <v>1</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40">
         <v>0.9</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40">
         <v>17</v>
       </c>
       <c r="I40">
@@ -11390,10 +11460,10 @@
       <c r="C41" s="2">
         <v>1</v>
       </c>
-      <c r="G41" s="3">
-        <v>1</v>
-      </c>
-      <c r="H41" s="4">
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
         <v>32</v>
       </c>
       <c r="I41">
@@ -11411,10 +11481,10 @@
       <c r="C42" s="2">
         <v>1</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="3">
         <f>SUM(H31:H41)</f>
         <v>54</v>
       </c>
@@ -11451,13 +11521,13 @@
       <c r="C45" s="2">
         <v>1</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G45" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I45" s="7" t="s">
+      <c r="I45" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -11471,10 +11541,10 @@
       <c r="C46" s="2">
         <v>1</v>
       </c>
-      <c r="G46" s="3">
-        <v>0</v>
-      </c>
-      <c r="H46" s="4">
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
         <v>0</v>
       </c>
       <c r="I46">
@@ -11491,10 +11561,10 @@
       <c r="C47" s="2">
         <v>1</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47">
         <v>0.1</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47">
         <v>0</v>
       </c>
       <c r="I47">
@@ -11511,10 +11581,10 @@
       <c r="C48" s="2">
         <v>1</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48">
         <v>0.2</v>
       </c>
-      <c r="H48" s="4">
+      <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
@@ -11531,10 +11601,10 @@
       <c r="C49" s="2">
         <v>1</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49">
         <v>0.3</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49">
         <v>0</v>
       </c>
       <c r="I49">
@@ -11551,10 +11621,10 @@
       <c r="C50" s="2">
         <v>1</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50">
         <v>0.4</v>
       </c>
-      <c r="H50" s="4">
+      <c r="H50">
         <v>0</v>
       </c>
       <c r="I50">
@@ -11571,10 +11641,10 @@
       <c r="C51" s="2">
         <v>1</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51">
         <v>0.5</v>
       </c>
-      <c r="H51" s="4">
+      <c r="H51">
         <v>0</v>
       </c>
       <c r="I51">
@@ -11591,10 +11661,10 @@
       <c r="C52" s="2">
         <v>1</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52">
         <v>0.6</v>
       </c>
-      <c r="H52" s="4">
+      <c r="H52">
         <v>0</v>
       </c>
       <c r="I52">
@@ -11611,10 +11681,10 @@
       <c r="C53" s="2">
         <v>1</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53">
         <v>0.7</v>
       </c>
-      <c r="H53" s="4">
+      <c r="H53">
         <v>0</v>
       </c>
       <c r="I53">
@@ -11631,10 +11701,10 @@
       <c r="C54" s="2">
         <v>1</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54">
         <v>0.8</v>
       </c>
-      <c r="H54" s="4">
+      <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
@@ -11643,7 +11713,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>0.26818675352877303</v>
+        <v>0.38487536966624403</v>
       </c>
       <c r="B55" s="2">
         <v>0.27904451682953302</v>
@@ -11651,10 +11721,10 @@
       <c r="C55" s="2">
         <v>1</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55">
         <v>0.9</v>
       </c>
-      <c r="H55" s="4">
+      <c r="H55">
         <v>0</v>
       </c>
       <c r="I55">
@@ -11664,10 +11734,10 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
-      <c r="G56" s="3">
-        <v>1</v>
-      </c>
-      <c r="H56" s="4">
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
         <v>54</v>
       </c>
       <c r="I56">
@@ -11677,10 +11747,10 @@
     <row r="57" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
-      <c r="G57" s="5" t="s">
+      <c r="G57" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H57" s="5">
+      <c r="H57" s="3">
         <f>SUM(H46:H56)</f>
         <v>54</v>
       </c>
@@ -11696,7 +11766,7 @@
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
-      <c r="G60" s="6" t="s">
+      <c r="G60" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H60" t="s">
@@ -11705,19 +11775,19 @@
       <c r="I60" t="s">
         <v>15</v>
       </c>
-      <c r="J60" s="7" t="s">
+      <c r="J60" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
-      <c r="G61" s="3">
+      <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
         <f ca="1">($H61/$H$27)*100</f>
-        <v>3.7037037037037033</v>
+        <v>3.6363636363636362</v>
       </c>
       <c r="I61">
         <f ca="1">($H61/$H$42)*100</f>
@@ -11730,7 +11800,7 @@
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="G62" s="3">
+      <c r="G62">
         <v>0.1</v>
       </c>
       <c r="H62">
@@ -11748,7 +11818,7 @@
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
-      <c r="G63" s="3">
+      <c r="G63">
         <v>0.2</v>
       </c>
       <c r="H63">
@@ -11766,12 +11836,12 @@
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
-      <c r="G64" s="3">
+      <c r="G64">
         <v>0.3</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7037037037037033</v>
+        <v>3.6363636363636362</v>
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="3"/>
@@ -11784,12 +11854,12 @@
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
-      <c r="G65" s="3">
+      <c r="G65">
         <v>0.4</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="2"/>
-        <v>14.814814814814813</v>
+        <v>16.363636363636363</v>
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="3"/>
@@ -11802,12 +11872,12 @@
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
-      <c r="G66" s="3">
+      <c r="G66">
         <v>0.5</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="2"/>
-        <v>62.962962962962962</v>
+        <v>61.818181818181813</v>
       </c>
       <c r="I66">
         <f t="shared" ca="1" si="3"/>
@@ -11820,12 +11890,12 @@
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
-      <c r="G67" s="3">
+      <c r="G67">
         <v>0.6</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="2"/>
-        <v>9.2592592592592595</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="3"/>
@@ -11838,7 +11908,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
-      <c r="G68" s="3">
+      <c r="G68">
         <v>0.7</v>
       </c>
       <c r="H68">
@@ -11856,7 +11926,7 @@
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
-      <c r="G69" s="3">
+      <c r="G69">
         <v>0.8</v>
       </c>
       <c r="H69">
@@ -11874,7 +11944,7 @@
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
-      <c r="G70" s="3">
+      <c r="G70">
         <v>0.9</v>
       </c>
       <c r="H70">
@@ -11892,12 +11962,12 @@
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
-      <c r="G71" s="3">
+      <c r="G71">
         <v>1</v>
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5555555555555554</v>
+        <v>5.4545454545454541</v>
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="3"/>
@@ -13140,8 +13210,8 @@
       <c r="B379" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G46:G56">
-    <sortCondition ref="G46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L16:L26">
+    <sortCondition ref="L16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13356,10 +13426,10 @@
       <c r="C14" s="2">
         <v>0.47996589940324003</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H14" t="s">
@@ -13376,10 +13446,10 @@
       <c r="C15" s="2">
         <v>0.51310861423220999</v>
       </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>2</v>
       </c>
       <c r="H15">
@@ -13397,10 +13467,10 @@
       <c r="C16" s="2">
         <v>0.49245063879210199</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>0.1</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
@@ -13418,10 +13488,10 @@
       <c r="C17" s="2">
         <v>0.47299382716049398</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <v>0.2</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
@@ -13439,10 +13509,10 @@
       <c r="C18" s="2">
         <v>0.37757667169431902</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>0.3</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18">
         <v>1</v>
       </c>
       <c r="H18">
@@ -13460,10 +13530,10 @@
       <c r="C19" s="2">
         <v>0.42044134727061599</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <v>0.4</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19">
         <v>11</v>
       </c>
       <c r="H19">
@@ -13481,10 +13551,10 @@
       <c r="C20" s="2">
         <v>0.29247067726068898</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20">
         <v>0.5</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20">
         <v>228</v>
       </c>
       <c r="H20">
@@ -13502,10 +13572,10 @@
       <c r="C21" s="2">
         <v>0.39743589743589702</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21">
         <v>0.6</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21">
         <v>16</v>
       </c>
       <c r="H21">
@@ -13523,10 +13593,10 @@
       <c r="C22" s="2">
         <v>0.44230769230769201</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22">
         <v>0.7</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22">
         <v>56</v>
       </c>
       <c r="H22">
@@ -13544,10 +13614,10 @@
       <c r="C23" s="2">
         <v>0.50418160095579501</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23">
         <v>0.8</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
@@ -13565,10 +13635,10 @@
       <c r="C24" s="2">
         <v>0.44102564102564101</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24">
         <v>0.9</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24">
         <v>4</v>
       </c>
       <c r="H24">
@@ -13586,10 +13656,10 @@
       <c r="C25" s="2">
         <v>0.49361207897793302</v>
       </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="4">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
         <v>60</v>
       </c>
       <c r="H25">
@@ -13607,10 +13677,10 @@
       <c r="C26" s="2">
         <v>0.49361207897793302</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="3">
         <f>SUM(G15:G25)</f>
         <v>378</v>
       </c>
@@ -13647,10 +13717,10 @@
       <c r="C29" s="2">
         <v>0.95818815331010498</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H29" t="s">
@@ -13667,10 +13737,10 @@
       <c r="C30" s="2">
         <v>0.97374429223744297</v>
       </c>
-      <c r="F30" s="3">
-        <v>0</v>
-      </c>
-      <c r="G30" s="4">
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>147</v>
       </c>
       <c r="H30">
@@ -13688,10 +13758,10 @@
       <c r="C31" s="2">
         <v>0.46689895470383302</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31">
         <v>0.1</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
@@ -13709,10 +13779,10 @@
       <c r="C32" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32">
         <v>0.2</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
@@ -13730,10 +13800,10 @@
       <c r="C33" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33">
         <v>0.3</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33">
         <v>2</v>
       </c>
       <c r="H33">
@@ -13751,10 +13821,10 @@
       <c r="C34" s="2">
         <v>0.99303135888501703</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34">
         <v>0.4</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
@@ -13772,10 +13842,10 @@
       <c r="C35" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35">
         <v>0.5</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35">
         <v>121</v>
       </c>
       <c r="H35">
@@ -13793,10 +13863,10 @@
       <c r="C36" s="2">
         <v>0.898954703832753</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36">
         <v>0.6</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36">
         <v>10</v>
       </c>
       <c r="H36">
@@ -13814,10 +13884,10 @@
       <c r="C37" s="2">
         <v>0.90011614401858298</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37">
         <v>0.7</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37">
         <v>46</v>
       </c>
       <c r="H37">
@@ -13835,10 +13905,10 @@
       <c r="C38" s="2">
         <v>0.898954703832753</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38">
         <v>0.8</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
@@ -13856,10 +13926,10 @@
       <c r="C39" s="2">
         <v>0.60511033681765403</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39">
         <v>0.9</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39">
         <v>1</v>
       </c>
       <c r="H39">
@@ -13877,10 +13947,10 @@
       <c r="C40" s="2">
         <v>0.90011614401858298</v>
       </c>
-      <c r="F40" s="3">
-        <v>1</v>
-      </c>
-      <c r="G40" s="4">
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
         <v>51</v>
       </c>
       <c r="H40">
@@ -13898,10 +13968,10 @@
       <c r="C41" s="2">
         <v>0.989547038327526</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="3">
         <f>SUM(G30:G40)</f>
         <v>378</v>
       </c>
@@ -13938,10 +14008,10 @@
       <c r="C44" s="2">
         <v>0.63879210220673599</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F44" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="G44" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H44" t="s">
@@ -13958,10 +14028,10 @@
       <c r="C45" s="2">
         <v>0.49825783972125398</v>
       </c>
-      <c r="F45" s="3">
-        <v>0</v>
-      </c>
-      <c r="G45" s="4">
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
@@ -13979,10 +14049,10 @@
       <c r="C46" s="2">
         <v>0.99070847851335697</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46">
         <v>0.1</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
@@ -14000,10 +14070,10 @@
       <c r="C47" s="2">
         <v>0.63879210220673599</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47">
         <v>0.2</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
@@ -14021,10 +14091,10 @@
       <c r="C48" s="2">
         <v>0.99767711962833905</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48">
         <v>0.3</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48">
         <v>1</v>
       </c>
       <c r="H48">
@@ -14042,10 +14112,10 @@
       <c r="C49" s="2">
         <v>0.99651567944250896</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49">
         <v>0.4</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49">
         <v>13</v>
       </c>
       <c r="H49">
@@ -14063,10 +14133,10 @@
       <c r="C50" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50">
         <v>0.5</v>
       </c>
-      <c r="G50" s="4">
+      <c r="G50">
         <v>177</v>
       </c>
       <c r="H50">
@@ -14084,10 +14154,10 @@
       <c r="C51" s="2">
         <v>0.47502903600464602</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51">
         <v>0.6</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51">
         <v>16</v>
       </c>
       <c r="H51">
@@ -14105,10 +14175,10 @@
       <c r="C52" s="2">
         <v>0.449477351916376</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52">
         <v>0.7</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52">
         <v>83</v>
       </c>
       <c r="H52">
@@ -14126,10 +14196,10 @@
       <c r="C53" s="2">
         <v>0.63995354239256697</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53">
         <v>0.8</v>
       </c>
-      <c r="G53" s="4">
+      <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
@@ -14147,10 +14217,10 @@
       <c r="C54" s="2">
         <v>0.49941927990708501</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54">
         <v>0.9</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54">
         <v>4</v>
       </c>
       <c r="H54">
@@ -14168,10 +14238,10 @@
       <c r="C55" s="2">
         <v>0.63763066202090601</v>
       </c>
-      <c r="F55" s="3">
-        <v>1</v>
-      </c>
-      <c r="G55" s="4">
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
         <v>84</v>
       </c>
       <c r="H55">
@@ -14189,10 +14259,10 @@
       <c r="C56" s="2">
         <v>0.63879210220673599</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="3">
         <f>SUM(G45:G55)</f>
         <v>378</v>
       </c>
@@ -14229,7 +14299,7 @@
       <c r="C59" s="2">
         <v>0.90243902439024404</v>
       </c>
-      <c r="F59" s="6" t="s">
+      <c r="F59" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G59" t="s">
@@ -14252,7 +14322,7 @@
       <c r="C60" s="2">
         <v>0.63879210220673599</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60">
         <v>0</v>
       </c>
       <c r="G60">
@@ -14278,7 +14348,7 @@
       <c r="C61" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61">
         <v>0.1</v>
       </c>
       <c r="G61">
@@ -14304,7 +14374,7 @@
       <c r="C62" s="2">
         <v>0.989547038327526</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F62">
         <v>0.2</v>
       </c>
       <c r="G62">
@@ -14330,7 +14400,7 @@
       <c r="C63" s="2">
         <v>0.49941927990708501</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63">
         <v>0.3</v>
       </c>
       <c r="G63">
@@ -14356,7 +14426,7 @@
       <c r="C64" s="2">
         <v>0.47038327526132401</v>
       </c>
-      <c r="F64" s="3">
+      <c r="F64">
         <v>0.4</v>
       </c>
       <c r="G64">
@@ -14382,7 +14452,7 @@
       <c r="C65" s="2">
         <v>0.49012775842044098</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65">
         <v>0.5</v>
       </c>
       <c r="G65">
@@ -14408,7 +14478,7 @@
       <c r="C66" s="2">
         <v>0.41811846689895499</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F66">
         <v>0.6</v>
       </c>
       <c r="G66">
@@ -14434,7 +14504,7 @@
       <c r="C67" s="2">
         <v>0.63879210220673599</v>
       </c>
-      <c r="F67" s="3">
+      <c r="F67">
         <v>0.7</v>
       </c>
       <c r="G67">
@@ -14460,7 +14530,7 @@
       <c r="C68" s="2">
         <v>0.50129870129870102</v>
       </c>
-      <c r="F68" s="3">
+      <c r="F68">
         <v>0.8</v>
       </c>
       <c r="G68">
@@ -14486,7 +14556,7 @@
       <c r="C69" s="2">
         <v>0.99535423925667799</v>
       </c>
-      <c r="F69" s="3">
+      <c r="F69">
         <v>0.9</v>
       </c>
       <c r="G69">
@@ -14512,7 +14582,7 @@
       <c r="C70" s="2">
         <v>0.99186991869918695</v>
       </c>
-      <c r="F70" s="3">
+      <c r="F70">
         <v>1</v>
       </c>
       <c r="G70">
@@ -17940,7 +18010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5B9A81-3CFA-FA47-9F67-64B54E5D0248}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
@@ -18143,10 +18213,10 @@
       <c r="C14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G14" t="s">
@@ -18163,10 +18233,10 @@
       <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
@@ -18184,10 +18254,10 @@
       <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
         <v>0.1</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16">
         <v>2</v>
       </c>
       <c r="G16">
@@ -18205,10 +18275,10 @@
       <c r="C17" s="2">
         <v>1</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>0.2</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17">
         <v>2</v>
       </c>
       <c r="G17">
@@ -18226,10 +18296,10 @@
       <c r="C18" s="2">
         <v>1</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>0.3</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18">
         <v>2</v>
       </c>
       <c r="G18">
@@ -18247,10 +18317,10 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>0.4</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19">
         <v>9</v>
       </c>
       <c r="G19">
@@ -18268,10 +18338,10 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20">
         <v>0.5</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20">
         <v>90</v>
       </c>
       <c r="G20">
@@ -18289,10 +18359,10 @@
       <c r="C21" s="2">
         <v>1</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
         <v>0.6</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21">
         <v>2</v>
       </c>
       <c r="G21">
@@ -18310,10 +18380,10 @@
       <c r="C22" s="2">
         <v>1</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
         <v>0.7</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
@@ -18331,10 +18401,10 @@
       <c r="C23" s="2">
         <v>1</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
         <v>0.8</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
@@ -18352,10 +18422,10 @@
       <c r="C24" s="2">
         <v>1</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24">
         <v>0.9</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
@@ -18373,10 +18443,10 @@
       <c r="C25" s="2">
         <v>1</v>
       </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
         <v>33</v>
       </c>
       <c r="G25">
@@ -18394,10 +18464,10 @@
       <c r="C26" s="2">
         <v>1</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="3">
         <f>SUM(F15:F25)</f>
         <v>141</v>
       </c>
@@ -18434,10 +18504,10 @@
       <c r="C29" s="2">
         <v>1</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G29" t="s">
@@ -18454,10 +18524,10 @@
       <c r="C30" s="2">
         <v>1</v>
       </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="4">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
@@ -18475,10 +18545,10 @@
       <c r="C31" s="2">
         <v>1</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31">
         <v>0.1</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31">
         <v>4</v>
       </c>
       <c r="G31">
@@ -18496,10 +18566,10 @@
       <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
         <v>0.2</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32">
         <v>0</v>
       </c>
       <c r="G32">
@@ -18517,10 +18587,10 @@
       <c r="C33" s="2">
         <v>1</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33">
         <v>0.3</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33">
         <v>2</v>
       </c>
       <c r="G33">
@@ -18538,10 +18608,10 @@
       <c r="C34" s="2">
         <v>1</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34">
         <v>0.4</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
@@ -18559,10 +18629,10 @@
       <c r="C35" s="2">
         <v>1</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35">
         <v>0.5</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35">
         <v>4</v>
       </c>
       <c r="G35">
@@ -18580,10 +18650,10 @@
       <c r="C36" s="2">
         <v>1</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36">
         <v>0.6</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36">
         <v>1</v>
       </c>
       <c r="G36">
@@ -18601,10 +18671,10 @@
       <c r="C37" s="2">
         <v>1</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37">
         <v>0.7</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37">
         <v>8</v>
       </c>
       <c r="G37">
@@ -18622,10 +18692,10 @@
       <c r="C38" s="2">
         <v>1</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38">
         <v>0.8</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38">
         <v>26</v>
       </c>
       <c r="G38">
@@ -18643,10 +18713,10 @@
       <c r="C39" s="2">
         <v>1</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39">
         <v>0.9</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39">
         <v>25</v>
       </c>
       <c r="G39">
@@ -18664,10 +18734,10 @@
       <c r="C40" s="2">
         <v>1</v>
       </c>
-      <c r="E40" s="3">
-        <v>1</v>
-      </c>
-      <c r="F40" s="4">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
         <v>71</v>
       </c>
       <c r="G40">
@@ -18685,10 +18755,10 @@
       <c r="C41" s="2">
         <v>1</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="3">
         <f>SUM(F30:F40)</f>
         <v>141</v>
       </c>
@@ -18714,10 +18784,10 @@
       <c r="C43" s="2">
         <v>1</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G43" t="s">
@@ -18734,10 +18804,10 @@
       <c r="C44" s="2">
         <v>1</v>
       </c>
-      <c r="E44" s="3">
-        <v>0</v>
-      </c>
-      <c r="F44" s="4">
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
         <v>0</v>
       </c>
       <c r="G44">
@@ -18755,10 +18825,10 @@
       <c r="C45" s="2">
         <v>1</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45">
         <v>0.1</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45">
         <v>0</v>
       </c>
       <c r="G45">
@@ -18776,10 +18846,10 @@
       <c r="C46" s="2">
         <v>1</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46">
         <v>0.2</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
@@ -18797,10 +18867,10 @@
       <c r="C47" s="2">
         <v>1</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47">
         <v>0.3</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47">
         <v>0</v>
       </c>
       <c r="G47">
@@ -18818,10 +18888,10 @@
       <c r="C48" s="2">
         <v>1</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48">
         <v>0.4</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
@@ -18839,10 +18909,10 @@
       <c r="C49" s="2">
         <v>1</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49">
         <v>0.5</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49">
         <v>0</v>
       </c>
       <c r="G49">
@@ -18860,10 +18930,10 @@
       <c r="C50" s="2">
         <v>1</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50">
         <v>0.6</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F50">
         <v>0</v>
       </c>
       <c r="G50">
@@ -18881,10 +18951,10 @@
       <c r="C51" s="2">
         <v>1</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51">
         <v>0.7</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
@@ -18902,10 +18972,10 @@
       <c r="C52" s="2">
         <v>1</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52">
         <v>0.8</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F52">
         <v>0</v>
       </c>
       <c r="G52">
@@ -18923,10 +18993,10 @@
       <c r="C53" s="2">
         <v>1</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53">
         <v>0.9</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53">
         <v>0</v>
       </c>
       <c r="G53">
@@ -18944,10 +19014,10 @@
       <c r="C54" s="2">
         <v>1</v>
       </c>
-      <c r="E54" s="3">
-        <v>1</v>
-      </c>
-      <c r="F54" s="4">
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
         <v>141</v>
       </c>
       <c r="G54">
@@ -18965,10 +19035,10 @@
       <c r="C55" s="2">
         <v>1</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F55" s="5">
+      <c r="F55" s="3">
         <f>SUM(F44:F54)</f>
         <v>141</v>
       </c>
@@ -18994,7 +19064,7 @@
       <c r="C57" s="2">
         <v>1</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F57" t="s">
@@ -19017,7 +19087,7 @@
       <c r="C58" s="2">
         <v>1</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
@@ -19043,7 +19113,7 @@
       <c r="C59" s="2">
         <v>1</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59">
         <v>0.1</v>
       </c>
       <c r="F59">
@@ -19069,7 +19139,7 @@
       <c r="C60" s="2">
         <v>1</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60">
         <v>0.2</v>
       </c>
       <c r="F60">
@@ -19095,7 +19165,7 @@
       <c r="C61" s="2">
         <v>1</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61">
         <v>0.3</v>
       </c>
       <c r="F61">
@@ -19121,7 +19191,7 @@
       <c r="C62" s="2">
         <v>1</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62">
         <v>0.4</v>
       </c>
       <c r="F62">
@@ -19147,7 +19217,7 @@
       <c r="C63" s="2">
         <v>1</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63">
         <v>0.5</v>
       </c>
       <c r="F63">
@@ -19173,7 +19243,7 @@
       <c r="C64" s="2">
         <v>1</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64">
         <v>0.6</v>
       </c>
       <c r="F64">
@@ -19199,7 +19269,7 @@
       <c r="C65" s="2">
         <v>1</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65">
         <v>0.7</v>
       </c>
       <c r="F65">
@@ -19225,7 +19295,7 @@
       <c r="C66" s="2">
         <v>1</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66">
         <v>0.8</v>
       </c>
       <c r="F66">
@@ -19251,7 +19321,7 @@
       <c r="C67" s="2">
         <v>1</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67">
         <v>0.9</v>
       </c>
       <c r="F67">
@@ -19277,7 +19347,7 @@
       <c r="C68" s="2">
         <v>1</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68">
         <v>1</v>
       </c>
       <c r="F68">

</xml_diff>